<commit_message>
New version of the Sierra Boyera Notebook
</commit_message>
<xml_diff>
--- a/data/rain.xlsx
+++ b/data/rain.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucordoba-my.sharepoint.com/personal/apenuela_uco_es/Documents/Master Hidraulica Ambiental/Planificacion/Notebooks/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andro\OneDrive - Universidad de Córdoba\Master Hidraulica Ambiental\Planificacion\Notebooks\MHA-Planificacion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A11084F0-E24B-4FB1-B1C6-A92C0E60244F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFF43017-5A53-4B60-BB8A-94E0AD7A5173}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01612A2A-77F7-4852-92A9-84E5EDBCE5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3846A3B-1B31-4DBC-84D0-420319BEFCCF}"/>
   </bookViews>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>fecha</t>
+    <t>date</t>
   </si>
   <si>
-    <t>precipitacion</t>
+    <t>precipitation</t>
   </si>
 </sst>
 </file>
@@ -141,14 +141,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,7 +182,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -292,7 +288,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,7 +430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2CBF02-CA5B-4F6C-BC6B-6B80B626AA0D}">
   <dimension ref="A1:B2703"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2680" workbookViewId="0">
-      <selection activeCell="E2968" sqref="E2968"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>